<commit_message>
Subiendo proyecto web, planilla testing y actualizando trello y product backlog
</commit_message>
<xml_diff>
--- a/Definition_Of_Done_DoD.xlsx
+++ b/Definition_Of_Done_DoD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Desktop\s3 ingenieria software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2D21DE4-ECCA-48FE-AFCE-90CA14F70185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74445393-ADDB-4148-B1FD-FC3BA691E56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1845" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -713,22 +713,37 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="5" fillId="13" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="14" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="14" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="9" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="14" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -739,13 +754,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
@@ -762,35 +771,26 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="9" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="5" fillId="13" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="14" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="14" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="14" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -898,10 +898,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -1419,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R992"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1452,25 +1452,25 @@
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:18" ht="27.75" customHeight="1">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="24" t="s">
         <v>38</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E2" s="5"/>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="35"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="38"/>
       <c r="L2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1485,23 +1485,23 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="51.75" customHeight="1">
-      <c r="A3" s="15"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="36">
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="15">
         <f>SUM(D2:D5)/12</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>9</v>
@@ -1517,23 +1517,23 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="26.25" customHeight="1">
-      <c r="A4" s="15"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="36">
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="15">
         <f>SUM(D6:D9)/12</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="8">
         <v>0</v>
@@ -1549,114 +1549,114 @@
       </c>
     </row>
     <row r="5" spans="1:18" ht="51.75" customHeight="1">
-      <c r="A5" s="15"/>
-      <c r="B5" s="23"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="33" t="s">
+      <c r="F5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="36">
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="15">
         <f>SUM(D10:D13)/12</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="45" customHeight="1">
-      <c r="A6" s="15"/>
-      <c r="B6" s="21" t="s">
+      <c r="A6" s="35"/>
+      <c r="B6" s="24" t="s">
         <v>39</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="36">
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="15">
         <f>SUM(D14,D17)/6</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="41.25" customHeight="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="22"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="36">
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="15">
         <f>SUM(D15,D18)/6</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="42.75" customHeight="1">
-      <c r="A8" s="15"/>
-      <c r="B8" s="22"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="38">
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="17">
         <f>SUM(D22:D25)/12</f>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="R8" s="32">
+        <v>1</v>
+      </c>
+      <c r="R8" s="14">
         <f>AVERAGE(I3:I6)</f>
-        <v>0.58333333333333326</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="30.75" customHeight="1">
-      <c r="A9" s="15"/>
-      <c r="B9" s="23"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="38">
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="17">
         <f>SUM(D26:D29)/12</f>
-        <v>0.41666666666666669</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="41.25" customHeight="1">
-      <c r="A10" s="15"/>
-      <c r="B10" s="21" t="s">
+      <c r="A10" s="35"/>
+      <c r="B10" s="24" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1666,19 +1666,19 @@
         <v>3</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="33" t="s">
+      <c r="F10" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="38">
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="17">
         <f>SUM(D30:D33)/12</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="47.25" customHeight="1">
-      <c r="A11" s="15"/>
-      <c r="B11" s="22"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="3" t="s">
         <v>8</v>
       </c>
@@ -1686,19 +1686,19 @@
         <v>3</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="38">
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="17">
         <f>SUM(D34:D37)/12</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="27.75" customHeight="1">
-      <c r="A12" s="15"/>
-      <c r="B12" s="22"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1706,38 +1706,38 @@
         <v>3</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="33" t="s">
+      <c r="F12" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="38">
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="50.25" customHeight="1">
-      <c r="A13" s="15"/>
-      <c r="B13" s="23"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="4">
         <v>3</v>
       </c>
-      <c r="F13" s="33" t="s">
+      <c r="F13" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="37">
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="16">
         <f>SUM(D42:D45)/12</f>
         <v>0</v>
       </c>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:18" ht="40.5" customHeight="1">
-      <c r="A14" s="15"/>
-      <c r="B14" s="21" t="s">
+      <c r="A14" s="35"/>
+      <c r="B14" s="24" t="s">
         <v>41</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1746,407 +1746,407 @@
       <c r="D14" s="4">
         <v>3</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="37">
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="16">
         <f>SUM(D46:D49)/12</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:18" ht="27.75" customHeight="1">
-      <c r="A15" s="15"/>
-      <c r="B15" s="22"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="25"/>
       <c r="C15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="4">
         <v>3</v>
       </c>
-      <c r="F15" s="33" t="s">
+      <c r="F15" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="37">
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="16">
         <f>SUM(D50:D53)/12</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:18" ht="36.75" customHeight="1">
-      <c r="A16" s="15"/>
-      <c r="B16" s="22"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="4">
         <v>3</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="37">
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="16">
         <f>SUM(D54:D57)/12</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="64.5" customHeight="1">
-      <c r="A17" s="15"/>
-      <c r="B17" s="23"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="4">
         <v>3</v>
       </c>
-      <c r="F17" s="33" t="s">
+      <c r="F17" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="37">
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="16">
         <f>SUM(D58:D61)/12</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="24" t="s">
         <v>42</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="25">
-        <v>0</v>
-      </c>
-      <c r="F18" s="33" t="s">
+      <c r="D18" s="13">
+        <v>3</v>
+      </c>
+      <c r="F18" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="37">
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="16">
         <f>SUM(D62:D65)/12</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A19" s="26"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="25">
-        <v>2</v>
-      </c>
-      <c r="F19" s="33" t="s">
+      <c r="D19" s="13">
+        <v>3</v>
+      </c>
+      <c r="F19" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="37">
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="16">
         <f>SUM(D66:D69)/12</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" ht="15.6">
-      <c r="A20" s="26"/>
-      <c r="B20" s="22"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="13">
         <v>3</v>
       </c>
       <c r="E20" s="5"/>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="38">
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="17">
         <f>SUM(D70:D73)/12</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="133.80000000000001" customHeight="1">
-      <c r="A21" s="26"/>
-      <c r="B21" s="23"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="26"/>
       <c r="C21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="13">
+        <v>3</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="17">
         <v>0</v>
       </c>
-      <c r="F21" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="38">
+    </row>
+    <row r="22" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A22" s="34"/>
+      <c r="B22" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="13">
+        <v>3</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A22" s="26"/>
-      <c r="B22" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="25">
-        <v>0</v>
-      </c>
-      <c r="F22" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="38">
-        <v>0</v>
-      </c>
-    </row>
     <row r="23" spans="1:10" ht="15.6">
-      <c r="A23" s="26"/>
-      <c r="B23" s="22"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="25"/>
       <c r="C23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="25">
-        <v>2</v>
-      </c>
-      <c r="F23" s="33" t="s">
+      <c r="D23" s="13">
+        <v>3</v>
+      </c>
+      <c r="F23" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="38">
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A24" s="26"/>
-      <c r="B24" s="22"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="25"/>
       <c r="C24" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="25">
-        <v>3</v>
-      </c>
-      <c r="F24" s="40" t="s">
+      <c r="D24" s="13">
+        <v>3</v>
+      </c>
+      <c r="F24" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="38">
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="86.4" customHeight="1">
-      <c r="A25" s="26"/>
-      <c r="B25" s="23"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="26"/>
       <c r="C25" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="25">
-        <v>0</v>
-      </c>
-      <c r="F25" s="42" t="s">
+      <c r="D25" s="13">
+        <v>3</v>
+      </c>
+      <c r="F25" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="39">
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="18">
         <f>SUM(D:D)/(22*12)</f>
-        <v>0.26893939393939392</v>
+        <v>0.95454545454545459</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A26" s="26"/>
-      <c r="B26" s="21" t="s">
+      <c r="A26" s="34"/>
+      <c r="B26" s="24" t="s">
         <v>44</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="25">
-        <v>0</v>
+      <c r="D26" s="13">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A27" s="26"/>
-      <c r="B27" s="22"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="25"/>
       <c r="C27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="25">
-        <v>2</v>
+      <c r="D27" s="13">
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A28" s="26"/>
-      <c r="B28" s="22"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="25"/>
       <c r="C28" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="25">
+      <c r="D28" s="13">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="85.2" customHeight="1">
-      <c r="A29" s="26"/>
-      <c r="B29" s="23"/>
+      <c r="A29" s="34"/>
+      <c r="B29" s="26"/>
       <c r="C29" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="25">
-        <v>0</v>
+      <c r="D29" s="13">
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="24" t="s">
         <v>48</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A31" s="15"/>
-      <c r="B31" s="22"/>
+      <c r="A31" s="35"/>
+      <c r="B31" s="25"/>
       <c r="C31" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D31" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A32" s="15"/>
-      <c r="B32" s="22"/>
+      <c r="A32" s="35"/>
+      <c r="B32" s="25"/>
       <c r="C32" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="90.6" customHeight="1">
-      <c r="A33" s="15"/>
-      <c r="B33" s="23"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="26"/>
       <c r="C33" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D33" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A34" s="15"/>
-      <c r="B34" s="21" t="s">
+      <c r="A34" s="35"/>
+      <c r="B34" s="24" t="s">
         <v>49</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A35" s="15"/>
-      <c r="B35" s="22"/>
+      <c r="A35" s="35"/>
+      <c r="B35" s="25"/>
       <c r="C35" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D35" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A36" s="15"/>
-      <c r="B36" s="22"/>
+      <c r="A36" s="35"/>
+      <c r="B36" s="25"/>
       <c r="C36" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D36" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="90.6" customHeight="1">
-      <c r="A37" s="15"/>
-      <c r="B37" s="23"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A38" s="15"/>
-      <c r="B38" s="21" t="s">
+      <c r="A38" s="35"/>
+      <c r="B38" s="24" t="s">
         <v>50</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D38" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A39" s="15"/>
-      <c r="B39" s="22"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="25"/>
       <c r="C39" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D39" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A40" s="15"/>
-      <c r="B40" s="22"/>
+      <c r="A40" s="35"/>
+      <c r="B40" s="25"/>
       <c r="C40" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="85.8" customHeight="1">
-      <c r="A41" s="15"/>
-      <c r="B41" s="23"/>
+      <c r="A41" s="35"/>
+      <c r="B41" s="26"/>
       <c r="C41" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A42" s="15"/>
-      <c r="B42" s="21" t="s">
+      <c r="A42" s="35"/>
+      <c r="B42" s="24" t="s">
         <v>51</v>
       </c>
       <c r="C42" s="3" t="s">
@@ -2157,8 +2157,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A43" s="15"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="25"/>
       <c r="C43" s="3" t="s">
         <v>8</v>
       </c>
@@ -2167,8 +2167,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A44" s="15"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="25"/>
       <c r="C44" s="3" t="s">
         <v>13</v>
       </c>
@@ -2177,8 +2177,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="78.599999999999994" customHeight="1">
-      <c r="A45" s="15"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="3" t="s">
         <v>14</v>
       </c>
@@ -2187,473 +2187,473 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A46" s="14" t="s">
+      <c r="A46" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="21" t="s">
+      <c r="B46" s="24" t="s">
         <v>53</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A47" s="27"/>
-      <c r="B47" s="22"/>
+      <c r="A47" s="28"/>
+      <c r="B47" s="25"/>
       <c r="C47" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D47" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A48" s="27"/>
-      <c r="B48" s="22"/>
+      <c r="A48" s="28"/>
+      <c r="B48" s="25"/>
       <c r="C48" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D48" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="75" customHeight="1">
-      <c r="A49" s="27"/>
-      <c r="B49" s="23"/>
+      <c r="A49" s="28"/>
+      <c r="B49" s="26"/>
       <c r="C49" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D49" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A50" s="27"/>
-      <c r="B50" s="21" t="s">
+      <c r="A50" s="28"/>
+      <c r="B50" s="24" t="s">
         <v>54</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D50" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A51" s="27"/>
-      <c r="B51" s="22"/>
+      <c r="A51" s="28"/>
+      <c r="B51" s="25"/>
       <c r="C51" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D51" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A52" s="27"/>
-      <c r="B52" s="22"/>
+      <c r="A52" s="28"/>
+      <c r="B52" s="25"/>
       <c r="C52" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D52" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="64.2" customHeight="1">
-      <c r="A53" s="27"/>
-      <c r="B53" s="23"/>
+      <c r="A53" s="28"/>
+      <c r="B53" s="26"/>
       <c r="C53" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D53" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A54" s="27"/>
-      <c r="B54" s="21" t="s">
+      <c r="A54" s="28"/>
+      <c r="B54" s="24" t="s">
         <v>55</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D54" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A55" s="27"/>
-      <c r="B55" s="22"/>
+      <c r="A55" s="28"/>
+      <c r="B55" s="25"/>
       <c r="C55" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D55" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A56" s="27"/>
-      <c r="B56" s="22"/>
+      <c r="A56" s="28"/>
+      <c r="B56" s="25"/>
       <c r="C56" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D56" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="50.4" customHeight="1">
-      <c r="A57" s="27"/>
-      <c r="B57" s="23"/>
+      <c r="A57" s="28"/>
+      <c r="B57" s="26"/>
       <c r="C57" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D57" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A58" s="27"/>
-      <c r="B58" s="21" t="s">
+      <c r="A58" s="28"/>
+      <c r="B58" s="24" t="s">
         <v>56</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D58" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A59" s="27"/>
-      <c r="B59" s="22"/>
+      <c r="A59" s="28"/>
+      <c r="B59" s="25"/>
       <c r="C59" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D59" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A60" s="27"/>
-      <c r="B60" s="22"/>
+      <c r="A60" s="28"/>
+      <c r="B60" s="25"/>
       <c r="C60" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D60" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="71.400000000000006" customHeight="1">
-      <c r="A61" s="27"/>
-      <c r="B61" s="23"/>
+      <c r="A61" s="28"/>
+      <c r="B61" s="26"/>
       <c r="C61" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A62" s="27"/>
-      <c r="B62" s="21" t="s">
+      <c r="A62" s="28"/>
+      <c r="B62" s="24" t="s">
         <v>57</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D62" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A63" s="27"/>
-      <c r="B63" s="22"/>
+      <c r="A63" s="28"/>
+      <c r="B63" s="25"/>
       <c r="C63" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D63" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A64" s="27"/>
-      <c r="B64" s="22"/>
+      <c r="A64" s="28"/>
+      <c r="B64" s="25"/>
       <c r="C64" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D64" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="75" customHeight="1">
-      <c r="A65" s="27"/>
-      <c r="B65" s="23"/>
+      <c r="A65" s="28"/>
+      <c r="B65" s="26"/>
       <c r="C65" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D65" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A66" s="27"/>
-      <c r="B66" s="21" t="s">
+      <c r="A66" s="28"/>
+      <c r="B66" s="24" t="s">
         <v>58</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D66" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A67" s="27"/>
-      <c r="B67" s="22"/>
+      <c r="A67" s="28"/>
+      <c r="B67" s="25"/>
       <c r="C67" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D67" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A68" s="27"/>
-      <c r="B68" s="22"/>
+      <c r="A68" s="28"/>
+      <c r="B68" s="25"/>
       <c r="C68" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D68" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="74.400000000000006" customHeight="1">
-      <c r="A69" s="27"/>
-      <c r="B69" s="23"/>
+      <c r="A69" s="28"/>
+      <c r="B69" s="26"/>
       <c r="C69" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D69" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A70" s="31" t="s">
+      <c r="A70" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B70" s="28" t="s">
+      <c r="B70" s="29" t="s">
         <v>60</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D70" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A71" s="31"/>
-      <c r="B71" s="29"/>
+      <c r="A71" s="32"/>
+      <c r="B71" s="30"/>
       <c r="C71" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D71" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A72" s="31"/>
-      <c r="B72" s="29"/>
+      <c r="A72" s="32"/>
+      <c r="B72" s="30"/>
       <c r="C72" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D72" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="81.599999999999994" customHeight="1">
-      <c r="A73" s="31"/>
-      <c r="B73" s="30"/>
+      <c r="A73" s="32"/>
+      <c r="B73" s="31"/>
       <c r="C73" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D73" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A74" s="31"/>
-      <c r="B74" s="28" t="s">
+      <c r="A74" s="32"/>
+      <c r="B74" s="29" t="s">
         <v>61</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D74" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A75" s="31"/>
-      <c r="B75" s="29"/>
+      <c r="A75" s="32"/>
+      <c r="B75" s="30"/>
       <c r="C75" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D75" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A76" s="31"/>
-      <c r="B76" s="29"/>
+      <c r="A76" s="32"/>
+      <c r="B76" s="30"/>
       <c r="C76" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D76" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="94.8" customHeight="1">
-      <c r="A77" s="31"/>
-      <c r="B77" s="30"/>
+      <c r="A77" s="32"/>
+      <c r="B77" s="31"/>
       <c r="C77" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D77" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A78" s="31" t="s">
+      <c r="A78" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="B78" s="28" t="s">
+      <c r="B78" s="29" t="s">
         <v>62</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D78" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A79" s="31"/>
-      <c r="B79" s="29"/>
+      <c r="A79" s="32"/>
+      <c r="B79" s="30"/>
       <c r="C79" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D79" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A80" s="31"/>
-      <c r="B80" s="29"/>
+      <c r="A80" s="32"/>
+      <c r="B80" s="30"/>
       <c r="C80" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D80" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="106.8" customHeight="1">
-      <c r="A81" s="31"/>
-      <c r="B81" s="30"/>
+      <c r="A81" s="32"/>
+      <c r="B81" s="31"/>
       <c r="C81" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D81" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A82" s="31" t="s">
+      <c r="A82" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="B82" s="28" t="s">
+      <c r="B82" s="29" t="s">
         <v>64</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D82" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A83" s="31"/>
-      <c r="B83" s="29"/>
+      <c r="A83" s="32"/>
+      <c r="B83" s="30"/>
       <c r="C83" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D83" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A84" s="31"/>
-      <c r="B84" s="29"/>
+      <c r="A84" s="32"/>
+      <c r="B84" s="30"/>
       <c r="C84" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D84" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="74.400000000000006" customHeight="1">
-      <c r="A85" s="31"/>
-      <c r="B85" s="30"/>
+      <c r="A85" s="32"/>
+      <c r="B85" s="31"/>
       <c r="C85" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D85" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A86" s="31"/>
-      <c r="B86" s="28" t="s">
+      <c r="A86" s="32"/>
+      <c r="B86" s="29" t="s">
         <v>65</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D86" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A87" s="31"/>
-      <c r="B87" s="29"/>
+      <c r="A87" s="32"/>
+      <c r="B87" s="30"/>
       <c r="C87" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D87" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A88" s="31"/>
-      <c r="B88" s="29"/>
+      <c r="A88" s="32"/>
+      <c r="B88" s="30"/>
       <c r="C88" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D88" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="88.8" customHeight="1">
-      <c r="A89" s="31"/>
-      <c r="B89" s="30"/>
+      <c r="A89" s="32"/>
+      <c r="B89" s="31"/>
       <c r="C89" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D89" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15.75" customHeight="1"/>
@@ -3561,43 +3561,6 @@
     <row r="992" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="A46:A69"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="B74:B77"/>
-    <mergeCell ref="A70:A77"/>
-    <mergeCell ref="B78:B81"/>
-    <mergeCell ref="A78:A81"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="B86:B89"/>
-    <mergeCell ref="A82:A89"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A18:A29"/>
-    <mergeCell ref="A30:A45"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="B42:B45"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="B10:B13"/>
@@ -3614,6 +3577,43 @@
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="F12:H12"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="A18:A29"/>
+    <mergeCell ref="A30:A45"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="B78:B81"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="B86:B89"/>
+    <mergeCell ref="A82:A89"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="A46:A69"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="B74:B77"/>
+    <mergeCell ref="A70:A77"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F22:H22"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="1">
@@ -3644,41 +3644,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.6">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5" ht="14.4">
-      <c r="B2" s="19">
+      <c r="B2" s="41">
         <f>Checklist!I7</f>
-        <v>0.5</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
     </row>
     <row r="3" spans="1:5" ht="14.4">
-      <c r="B3" s="18"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="1:5" ht="14.4">
-      <c r="B4" s="18"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="40"/>
     </row>
     <row r="5" spans="1:5" ht="14.4">
-      <c r="B5" s="18"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="18"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="40"/>
     </row>
     <row r="6" spans="1:5" ht="14.4">
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -4693,15 +4693,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010070BFDEA41A5D8B46AA5DA2E2389CBE4E" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="672700c7c1e39a78a362f54b21ce1efa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d0daa353-f819-43d1-badf-ce69fea8800d" xmlns:ns3="edc1eb1c-f9b5-429a-a0ce-702847a0aa2d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3db37e5c6f54565a9911855e2c96e577" ns2:_="" ns3:_="">
     <xsd:import namespace="d0daa353-f819-43d1-badf-ce69fea8800d"/>
@@ -4956,6 +4947,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CD51195-12DE-4B0C-BEB4-16018FC7E2F0}">
   <ds:schemaRefs>
@@ -4968,14 +4968,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FA387EC-F6D6-4C39-850A-38D5ECF4D0D9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E14E2735-EA1A-44BF-9884-36133875E543}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4992,4 +4984,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FA387EC-F6D6-4C39-850A-38D5ECF4D0D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>